<commit_message>
clean up images- details
</commit_message>
<xml_diff>
--- a/Capstone 2/Reports/StatisticalResults.xlsx
+++ b/Capstone 2/Reports/StatisticalResults.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlinewing/Desktop/Capstone 2/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{553A7B1C-06CD-7246-9CBA-8EF5FF4BF6D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74620B43-5CF7-F342-B16B-A73E5E9DC930}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="2420" windowWidth="28040" windowHeight="16680" xr2:uid="{420EB4AE-B734-7B4C-8995-8F858B7F0D79}"/>
+    <workbookView xWindow="760" yWindow="520" windowWidth="28040" windowHeight="16680" xr2:uid="{420EB4AE-B734-7B4C-8995-8F858B7F0D79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -107,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -231,17 +231,18 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -249,7 +250,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,7 +573,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,17 +610,17 @@
     <row r="3" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -628,15 +628,15 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="1"/>
@@ -646,19 +646,19 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="6">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
         <v>1.8455000000000001E-38</v>
       </c>
       <c r="H5" s="1"/>
@@ -672,19 +672,19 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="6">
         <v>-4.3E-3</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5">
         <v>4.8694999999999999E-4</v>
       </c>
       <c r="H6" s="1"/>
@@ -694,19 +694,19 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="6">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5">
         <v>3.3714999999999998E-6</v>
       </c>
       <c r="H7" s="1"/>
@@ -716,19 +716,19 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="6">
         <v>-8.7000000000000001E-4</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>9.0660000000000004E-2</v>
       </c>
       <c r="H8" s="1"/>
@@ -738,19 +738,19 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="F9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5">
         <v>5.3680000000000004E-4</v>
       </c>
       <c r="H9" s="1"/>
@@ -760,19 +760,19 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="6">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="F10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="5">
         <v>2.0667000000000001E-6</v>
       </c>
       <c r="H10" s="1"/>
@@ -782,19 +782,19 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="F11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5">
         <v>9.3189000000000005E-5</v>
       </c>
       <c r="H11" s="1"/>
@@ -804,19 +804,19 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="6">
         <v>0.04</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="F12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="5">
         <v>1.0272999999999999E-21</v>
       </c>
       <c r="H12" s="1"/>
@@ -826,19 +826,19 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="6">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="F13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5">
         <v>1.268E-8</v>
       </c>
       <c r="H13" s="1"/>
@@ -848,19 +848,19 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="7">
+      <c r="F14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="5">
         <v>5.3109000000000003E-7</v>
       </c>
       <c r="H14" s="1"/>
@@ -870,19 +870,19 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="6">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="7">
+      <c r="F15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="5">
         <v>5.5153000000000003E-24</v>
       </c>
       <c r="H15" s="1"/>
@@ -892,19 +892,19 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="6">
         <v>0.05</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="7">
+      <c r="F16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="5">
         <v>8.8953000000000007E-12</v>
       </c>
       <c r="H16" s="1"/>
@@ -914,19 +914,19 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="7">
+      <c r="F17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="5">
         <v>4.4464E-4</v>
       </c>
       <c r="H17" s="1"/>
@@ -936,19 +936,19 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="6">
         <v>-7.9000000000000008E-3</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="5">
         <v>0.24679999999999999</v>
       </c>
       <c r="H18" s="1"/>
@@ -958,19 +958,19 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="6">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="7">
+      <c r="F19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="5">
         <v>3.4071E-6</v>
       </c>
       <c r="H19" s="1"/>
@@ -1063,5 +1063,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>